<commit_message>
Prions que ça marche
</commit_message>
<xml_diff>
--- a/mediafiles/izoua.xlsx
+++ b/mediafiles/izoua.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,47 +496,47 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Niarry Tally</t>
+          <t>Yoff</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17h00</t>
+          <t>05h26</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Cagil</t>
+          <t>Bazoungoula</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Livré</t>
+          <t>En attente</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Glenn</t>
+          <t>George N'gock</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Chez Izoua</t>
+          <t>Chez le livreur</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Vosgienne Taille Grande</t>
+          <t>Vosgienne Taille Petite, Vosgienne - Antoinette Taille Grande</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>2000</v>
+        <v>1200</v>
       </c>
       <c r="K2" t="n">
-        <v>5000</v>
+        <v>7500</v>
       </c>
       <c r="L2" t="n">
-        <v>7000</v>
+        <v>8700</v>
       </c>
     </row>
     <row r="3">
@@ -547,52 +547,110 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Oui</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Commandée sur place</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Heure sur place: 12:09</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Commandée sur place</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Sur place</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Coulibaly Yelanto</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Chez Izoua</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Antoinette Taille Petite</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Commandée sur place</t>
+        </is>
+      </c>
+      <c r="K3" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L3" t="n">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>27 décembre 2024</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>Non</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Liberté 1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>01h26</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Bazoungoula</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Ouest Foire Dakar</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>02h51</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Cagil</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>Livré</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Amos</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>yve kate</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>Chez le livreur</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Selucy Taille Petite Supplements: Fromages, Crème fraiche, Lardons, LA FERMIERE DE MAMAN ISA Taille Grande</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>1500</v>
-      </c>
-      <c r="K3" t="n">
-        <v>10140</v>
-      </c>
-      <c r="L3" t="n">
-        <v>11640</v>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Antoinette Taille Grande</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>900</v>
+      </c>
+      <c r="K4" t="n">
+        <v>5000</v>
+      </c>
+      <c r="L4" t="n">
+        <v>5900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dieu merci tout marche
</commit_message>
<xml_diff>
--- a/mediafiles/izoua.xlsx
+++ b/mediafiles/izoua.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,25 +459,30 @@
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Mode de paiement</t>
+          <t>Mode de paiement commandes</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>Mode de paiement livraison</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>Infos Pizzas</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Prix Livraison</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Prix Pizzas + Suppléments</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
@@ -491,32 +496,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Non</t>
+          <t>Oui</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Yoff</t>
+          <t>Commandée sur place</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>05h26</t>
+          <t>Heure sur place: 17:40</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Bazoungoula</t>
+          <t>Commandée sur place</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>En attente</t>
+          <t>Sur place</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>George N'gock</t>
+          <t>Lahat Samb</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -526,17 +531,22 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Vosgienne Taille Petite, Vosgienne - Antoinette Taille Grande</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>1200</v>
+          <t>Chez le livreur</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Selucy Taille Petite, Margherita - Vosgienne Taille Grande Supplements: Fromages, Emmental</t>
+        </is>
       </c>
       <c r="K2" t="n">
-        <v>7500</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>8700</v>
+        <v>9600</v>
+      </c>
+      <c r="M2" t="n">
+        <v>9600</v>
       </c>
     </row>
     <row r="3">
@@ -547,54 +557,59 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Oui</t>
+          <t>Non</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Ouest Foire Dakar</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>19h53</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Cagil</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Livré</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>George N'gock</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Chez Izoua</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Chez Izoua</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Selucy Taille Grande, Margherita - Vosgienne Taille Grande</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
           <t>Commandée sur place</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Heure sur place: 12:09</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Commandée sur place</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Sur place</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Coulibaly Yelanto</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Chez Izoua</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Antoinette Taille Petite</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Commandée sur place</t>
-        </is>
-      </c>
-      <c r="K3" t="n">
-        <v>2500</v>
-      </c>
       <c r="L3" t="n">
-        <v>2500</v>
+        <v>10000</v>
+      </c>
+      <c r="M3" t="n">
+        <v>11800</v>
       </c>
     </row>
     <row r="4">
@@ -610,17 +625,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Ouest Foire Dakar</t>
+          <t>Keur Gorgui</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>02h51</t>
+          <t>22h55</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Cagil</t>
+          <t>Bazoungoula</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -630,27 +645,160 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>yve kate</t>
+          <t>Coulibaly Yelanto</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Chez le livreur</t>
+          <t>Chez Izoua</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Antoinette Taille Grande</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>900</v>
-      </c>
-      <c r="K4" t="n">
-        <v>5000</v>
+          <t>Chez Izoua</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Vosgienne Taille Petite, Margherita - Selucy Taille Grande</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Commandée sur place</t>
+        </is>
       </c>
       <c r="L4" t="n">
-        <v>5900</v>
+        <v>7500</v>
+      </c>
+      <c r="M4" t="n">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>27 décembre 2024</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Ouest Foire</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>22h56</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Bazoungoula</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Annulé</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Yves</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Chez Izoua</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Chez Izoua</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Vosgienne - Selucy Taille Grande Supplements: Fromages, Emmental</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Commandée sur place</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>7100</v>
+      </c>
+      <c r="M5" t="n">
+        <v>9100</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>27 décembre 2024</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Non</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Grand Dakar</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>20h55</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Bazoungoula</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>En attente</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Alphonse Desire</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Chez Izoua</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Chez Izoua</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Selucy Taille Grande, Vosgienne - Margherita Taille Grande</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Commandée sur place</t>
+        </is>
+      </c>
+      <c r="L6" t="n">
+        <v>10000</v>
+      </c>
+      <c r="M6" t="n">
+        <v>11500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>